<commit_message>
rolled back incorrect display location kpi switched to using all_products for sos num not found. duh.
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="157">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t xml:space="preserve">Display by Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scene_fk</t>
   </si>
   <si>
     <t xml:space="preserve">POP Seasonal Programs</t>
@@ -418,19 +415,25 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
+    <t xml:space="preserve">Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Displays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POPs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCC Cooler</t>
+  </si>
+  <si>
     <t xml:space="preserve">Any</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Displays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POPs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCC Cooler</t>
   </si>
   <si>
     <t xml:space="preserve">Comparable Type</t>
@@ -522,7 +525,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -558,12 +561,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -712,12 +709,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -770,11 +767,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,15 +779,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -802,23 +795,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -917,19 +910,19 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="77.1255060728745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="77.7692307692308"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1491,10 +1484,10 @@
       <c r="G19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="10" t="s">
         <v>53</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -1504,44 +1497,40 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+    <row r="20" s="13" customFormat="true" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="J20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>52</v>
@@ -1552,7 +1541,7 @@
         <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>16</v>
@@ -1569,18 +1558,18 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="10" t="s">
         <v>14</v>
       </c>
@@ -1601,10 +1590,10 @@
     </row>
     <row r="23" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
@@ -1632,10 +1621,10 @@
     </row>
     <row r="24" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
@@ -1661,16 +1650,16 @@
     </row>
     <row r="25" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="10"/>
       <c r="F25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>16</v>
@@ -1694,15 +1683,15 @@
     </row>
     <row r="26" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="11"/>
       <c r="E26" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>25</v>
@@ -1711,13 +1700,13 @@
         <v>26</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1725,10 +1714,10 @@
     </row>
     <row r="27" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
@@ -1752,10 +1741,10 @@
     </row>
     <row r="28" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
@@ -1779,10 +1768,10 @@
     </row>
     <row r="29" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
@@ -1806,10 +1795,10 @@
     </row>
     <row r="30" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
@@ -1833,10 +1822,10 @@
     </row>
     <row r="31" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="11"/>
@@ -1860,10 +1849,10 @@
     </row>
     <row r="32" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="11"/>
@@ -1871,13 +1860,13 @@
         <v>50</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1887,10 +1876,10 @@
     </row>
     <row r="33" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
@@ -1898,13 +1887,13 @@
         <v>37</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1914,10 +1903,10 @@
     </row>
     <row r="34" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
@@ -1925,13 +1914,13 @@
         <v>31</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1941,10 +1930,10 @@
     </row>
     <row r="35" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
@@ -1952,13 +1941,13 @@
         <v>34</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1968,10 +1957,10 @@
     </row>
     <row r="36" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
@@ -1999,10 +1988,10 @@
     </row>
     <row r="37" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="11"/>
@@ -2030,10 +2019,10 @@
     </row>
     <row r="38" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="11"/>
@@ -2061,10 +2050,10 @@
     </row>
     <row r="39" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="11"/>
@@ -2092,10 +2081,10 @@
     </row>
     <row r="40" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="11"/>
@@ -2118,14 +2107,14 @@
       <c r="M40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="16"/>
+      <c r="A41" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15"/>
       <c r="E41" s="10" t="s">
         <v>37</v>
       </c>
@@ -2146,10 +2135,10 @@
     </row>
     <row r="42" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
@@ -2173,10 +2162,10 @@
     </row>
     <row r="43" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
@@ -2200,10 +2189,10 @@
     </row>
     <row r="44" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
@@ -2211,13 +2200,13 @@
         <v>50</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2227,10 +2216,10 @@
     </row>
     <row r="45" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="11"/>
@@ -2238,13 +2227,13 @@
         <v>37</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2254,10 +2243,10 @@
     </row>
     <row r="46" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="11"/>
@@ -2265,13 +2254,13 @@
         <v>31</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2281,10 +2270,10 @@
     </row>
     <row r="47" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
@@ -2292,13 +2281,13 @@
         <v>34</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2308,15 +2297,15 @@
     </row>
     <row r="48" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>96</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
       <c r="E48" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>15</v>
@@ -2361,8 +2350,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2370,16 +2359,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>130</v>
+      <c r="B1" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2406,9 +2395,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2416,34 +2405,34 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2470,9 +2459,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2481,118 +2470,118 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>134</v>
+      <c r="D1" s="16" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2660,10 +2649,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2672,27 +2661,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2723,184 +2712,184 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="24" t="n">
+      <c r="A3" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="n">
+      <c r="C3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="n">
+      <c r="D3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="24" t="n">
+      <c r="F3" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="n">
+      <c r="G3" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="24" t="n">
+      <c r="H3" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="I3" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="23" t="n">
         <v>9</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="23" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="n">
+      <c r="A4" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
+      <c r="C4" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="n">
+      <c r="A5" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="E6" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="D7" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="F7" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="G8" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2929,9 +2918,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2940,175 +2929,175 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>134</v>
+      <c r="D1" s="16" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" s="26"/>
+        <v>147</v>
+      </c>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3135,8 +3124,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3144,25 +3133,25 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>134</v>
+      <c r="D1" s="16" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -3217,10 +3206,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,12 +3217,12 @@
         <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>26</v>
@@ -3241,7 +3230,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -3249,12 +3238,12 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3281,11 +3270,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3293,17 +3282,17 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3311,11 +3300,11 @@
         <v>22</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -3324,11 +3313,11 @@
         <v>28</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="10"/>
     </row>
@@ -3356,11 +3345,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3368,17 +3357,17 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>106</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="49" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3386,13 +3375,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -3403,13 +3392,13 @@
         <v>32</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D3" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -3420,13 +3409,13 @@
         <v>33</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -3437,13 +3426,13 @@
         <v>35</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D5" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
@@ -3454,13 +3443,13 @@
         <v>36</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>1</v>
@@ -3471,13 +3460,13 @@
         <v>38</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="D7" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
@@ -3507,9 +3496,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3517,11 +3506,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>112</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3529,10 +3518,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3560,9 +3549,9 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3571,20 +3560,20 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3592,18 +3581,18 @@
         <v>48</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="18" t="n">
+      <c r="E2" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="19" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -3626,13 +3615,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3640,14 +3629,14 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3655,13 +3644,13 @@
         <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>124</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3669,37 +3658,37 @@
         <v>54</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>129</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3726,8 +3715,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3735,16 +3724,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>130</v>
+      <c r="B1" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3771,7 +3760,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
@@ -3780,8 +3769,8 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>120</v>
+      <c r="B1" s="16" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,22 +3813,22 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base measure, bay number
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,6 +25,8 @@
     <sheet name="Share of Shelf" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Purity" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Hierarchy" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Base Measurement" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Bay Count" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="159">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -95,7 +97,7 @@
     <t xml:space="preserve">template_fk</t>
   </si>
   <si>
-    <t xml:space="preserve">store_fk</t>
+    <t xml:space="preserve">store_id</t>
   </si>
   <si>
     <t xml:space="preserve">Molson Coors Cooler Exceptions</t>
@@ -515,6 +517,12 @@
   </si>
   <si>
     <t xml:space="preserve">POSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum Col</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net_len_ign_stack</t>
   </si>
 </sst>
 </file>
@@ -830,15 +838,33 @@
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -910,19 +936,19 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="78.412955465587"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="79.1619433198381"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2345,13 +2371,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N40" activeCellId="1" sqref="E2:E48 N40"/>
+      <selection pane="topLeft" activeCell="N40" activeCellId="0" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2390,14 +2416,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E2:E48 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2454,14 +2480,14 @@
   <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E2:E48 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2644,15 +2670,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="E2:E48 I11"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2703,7 +2729,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA29" activeCellId="1" sqref="E2:E48 AA29"/>
+      <selection pane="topLeft" activeCell="AA29" activeCellId="0" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2913,14 +2939,14 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="E2:E48 B21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -3119,13 +3145,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="E2:E48 B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3194,7 +3220,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z19" activeCellId="1" sqref="E2:E48 Z19"/>
+      <selection pane="topLeft" activeCell="Z19" activeCellId="0" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3244,6 +3270,115 @@
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W20" activeCellId="0" sqref="W20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0445344129555"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3265,16 +3400,16 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E2:E48"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3340,16 +3475,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="E2:E48 I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3491,14 +3626,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E48 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3543,15 +3678,15 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E48"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3615,13 +3750,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="1" sqref="E2:E48 P12"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3710,13 +3845,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="1" sqref="E2:E48 I16"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3755,12 +3890,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="E2:E48 F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
@@ -3800,7 +3935,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="1" sqref="E2:E48 J18"/>
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
added dynamic out of stock
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="161">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -441,7 +441,16 @@
     <t xml:space="preserve">Comparable Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Must-Have SKUs</t>
+    <t xml:space="preserve">Param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
   </si>
   <si>
     <t xml:space="preserve">Molson Coors </t>
@@ -511,9 +520,6 @@
   </si>
   <si>
     <t xml:space="preserve">Brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKU</t>
   </si>
   <si>
     <t xml:space="preserve">POSM</t>
@@ -533,7 +539,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -591,6 +597,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -717,12 +729,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -803,23 +815,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -838,33 +854,15 @@
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -936,19 +934,19 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="79.1619433198381"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="79.8016194331984"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2376,8 +2374,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2421,9 +2419,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2452,10 +2450,10 @@
         <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>69</v>
@@ -2485,9 +2483,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2503,7 +2501,7 @@
         <v>104</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2563,7 @@
         <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,7 +2577,7 @@
         <v>108</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2593,7 +2591,7 @@
         <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,7 +2605,7 @@
         <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2675,10 +2673,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2687,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>97</v>
@@ -2701,13 +2699,13 @@
         <v>94</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2738,184 +2736,184 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="A1" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="23" t="n">
+      <c r="A3" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="23" t="n">
+      <c r="F3" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="23" t="n">
+      <c r="G3" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="23" t="n">
+      <c r="H3" s="24" t="n">
         <v>7</v>
       </c>
-      <c r="I3" s="23" t="n">
+      <c r="I3" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="23" t="n">
+      <c r="J3" s="24" t="n">
         <v>9</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="24" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="n">
+      <c r="A4" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="B4" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="n">
+      <c r="A5" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="B5" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="n">
+      <c r="A6" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
+      <c r="C6" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="n">
+      <c r="A7" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="C7" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="n">
+      <c r="A8" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="G8" s="24" t="s">
+      <c r="B8" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="C8" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2944,9 +2942,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2962,7 +2960,7 @@
         <v>104</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2976,9 +2974,9 @@
         <v>108</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="25"/>
+        <v>150</v>
+      </c>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
@@ -2988,10 +2986,10 @@
         <v>107</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3002,10 +3000,10 @@
         <v>107</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3016,10 +3014,10 @@
         <v>107</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3081,7 +3079,7 @@
         <v>108</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,7 +3093,7 @@
         <v>108</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3109,7 +3107,7 @@
         <v>108</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3123,7 +3121,7 @@
         <v>108</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3150,8 +3148,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3166,7 +3164,7 @@
         <v>104</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,10 +3230,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,12 +3241,12 @@
         <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>26</v>
@@ -3256,7 +3254,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -3264,7 +3262,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,9 +3294,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6518218623482"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,23 +3312,23 @@
         <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>158</v>
+      <c r="B3" s="26" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>158</v>
+      <c r="B4" s="26" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3351,14 +3349,14 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0445344129555"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3399,17 +3397,17 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3480,11 +3478,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3631,9 +3629,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3684,9 +3682,9 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3755,8 +3753,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3850,8 +3848,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3895,7 +3893,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8502024291498"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
@@ -3932,38 +3930,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2672064777328"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>132</v>
       </c>
+      <c r="E1" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="B2" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>108</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched base measure over to mpis
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -528,7 +528,7 @@
     <t xml:space="preserve">Sum Col</t>
   </si>
   <si>
-    <t xml:space="preserve">net_len_ign_stack</t>
+    <t xml:space="preserve">width_mm_advance</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -597,12 +597,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -729,12 +723,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -815,27 +809,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -934,19 +924,19 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="1" sqref="B4 A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="80.4453441295547"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2369,13 +2359,13 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="B4 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2415,14 +2405,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2479,14 +2469,14 @@
   <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2669,15 +2659,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="B4 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2728,7 +2718,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA29" activeCellId="0" sqref="AA29"/>
+      <selection pane="topLeft" activeCell="AA29" activeCellId="1" sqref="B4 AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2737,184 +2727,184 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="24" t="n">
+      <c r="B3" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="n">
+      <c r="C3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="n">
+      <c r="D3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="24" t="n">
+      <c r="F3" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="n">
+      <c r="G3" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="24" t="n">
+      <c r="H3" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="I3" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="23" t="n">
         <v>9</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="23" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="n">
+      <c r="A4" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="n">
+      <c r="A5" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="n">
+      <c r="A6" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="n">
+      <c r="A7" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="n">
+      <c r="A8" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2938,14 +2928,14 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="B4 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2977,7 +2967,7 @@
       <c r="D2" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
@@ -3144,13 +3134,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="B4 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3219,7 +3209,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z19" activeCellId="0" sqref="Z19"/>
+      <selection pane="topLeft" activeCell="Z19" activeCellId="1" sqref="B4 Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3289,14 +3279,14 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W20" activeCellId="0" sqref="W20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3320,7 +3310,7 @@
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="0" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3328,7 +3318,7 @@
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="0" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3351,12 +3341,12 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3399,16 +3389,16 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="B4 E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3474,16 +3464,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="B4 I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3625,14 +3615,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B4 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.1336032388664"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3677,15 +3667,15 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="B4 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3749,13 +3739,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="1" sqref="B4 P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3844,13 +3834,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="1" sqref="B4 I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3889,12 +3879,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="B4 F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
@@ -3934,15 +3924,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="B4 G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2672064777328"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3964,7 +3954,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="10" t="s">

</xml_diff>

<commit_message>
product sequence partially implemented
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,9 +29,10 @@
     <sheet name="Bay Count" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="161">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -453,22 +454,13 @@
     <t xml:space="preserve">A Value 1</t>
   </si>
   <si>
-    <t xml:space="preserve">A Param 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Value 2</t>
+    <t xml:space="preserve">Iterative</t>
   </si>
   <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
     <t xml:space="preserve">Molson Coors </t>
-  </si>
-  <si>
-    <t xml:space="preserve">labels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iterative</t>
   </si>
   <si>
     <t xml:space="preserve">den_col</t>
@@ -941,13 +933,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="83.3400809716599"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="84.0890688259109"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="35.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2352,7 +2344,7 @@
       <c r="M48" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E48"/>
+  <autoFilter ref="A1:L48"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2377,8 +2369,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2426,21 +2418,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2453,24 +2445,18 @@
       <c r="D1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="10" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2498,9 +2484,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2516,7 +2502,7 @@
         <v>105</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,7 +2564,7 @@
         <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2578,7 @@
         <v>108</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,7 +2592,7 @@
         <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2606,7 @@
         <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2688,9 +2674,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2700,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>134</v>
@@ -2714,13 +2700,13 @@
         <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2752,10 +2738,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2782,7 +2768,7 @@
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="24" t="n">
         <v>1</v>
@@ -2820,10 +2806,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -2839,13 +2825,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -2860,16 +2846,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>149</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>152</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -2883,19 +2869,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>149</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>152</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -2908,22 +2894,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>149</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>152</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -2957,9 +2943,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2975,7 +2961,7 @@
         <v>105</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2989,7 +2975,7 @@
         <v>108</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F2" s="17"/>
     </row>
@@ -3001,10 +2987,10 @@
         <v>107</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3015,10 +3001,10 @@
         <v>107</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3029,10 +3015,10 @@
         <v>107</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3094,7 +3080,7 @@
         <v>108</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3108,7 +3094,7 @@
         <v>108</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3122,7 +3108,7 @@
         <v>108</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3136,7 +3122,7 @@
         <v>108</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3163,10 +3149,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3257,10 +3243,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3268,12 +3254,12 @@
         <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>25</v>
@@ -3289,7 +3275,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,8 +3307,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3331,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,7 +3325,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,7 +3333,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,7 +3341,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3382,7 +3368,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3430,10 +3416,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3525,11 +3511,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3676,9 +3662,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3712,16 +3698,16 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3790,8 +3776,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3873,8 +3859,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3918,8 +3904,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -3983,10 +3969,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
bug fixes eye level
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
     <sheet name="Share of Shelf" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Purity" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Hierarchy" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Base Measurement" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Linear Measurement" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Bay Count" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames>
@@ -34,6 +34,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="160">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -164,7 +166,7 @@
     <t xml:space="preserve">Warm Base Measurement</t>
   </si>
   <si>
-    <t xml:space="preserve">Base Measurement</t>
+    <t xml:space="preserve">Linear Measurement</t>
   </si>
   <si>
     <t xml:space="preserve">Session</t>
@@ -347,6 +349,9 @@
     <t xml:space="preserve">Flankers</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Competitive Brands</t>
   </si>
   <si>
@@ -413,7 +418,10 @@
     <t xml:space="preserve">Scored</t>
   </si>
   <si>
-    <t xml:space="preserve">Metric</t>
+    <t xml:space="preserve">Result Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score Metric</t>
   </si>
   <si>
     <t xml:space="preserve">Innovations</t>
@@ -425,15 +433,18 @@
     <t xml:space="preserve">Displays</t>
   </si>
   <si>
+    <t xml:space="preserve">Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POPs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count</t>
   </si>
   <si>
-    <t xml:space="preserve">POPs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
     <t xml:space="preserve">MCC Cooler</t>
   </si>
   <si>
@@ -452,9 +463,6 @@
     <t xml:space="preserve">Iterative</t>
   </si>
   <si>
-    <t xml:space="preserve">Manufacturer</t>
-  </si>
-  <si>
     <t xml:space="preserve">Molson Coors </t>
   </si>
   <si>
@@ -464,16 +472,10 @@
     <t xml:space="preserve">Business Question </t>
   </si>
   <si>
-    <t xml:space="preserve">A Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Value 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Are MCC Brands placed at Eye Level on shelf?</t>
   </si>
   <si>
-    <t xml:space="preserve">Molson coors </t>
+    <t xml:space="preserve">Eye</t>
   </si>
   <si>
     <t xml:space="preserve">When there are
@@ -489,9 +491,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bottom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eye</t>
   </si>
   <si>
     <t xml:space="preserve">Middle</t>
@@ -928,19 +927,19 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="84.8380566801619"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="86.336032388664"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2313,7 +2312,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
         <v>92</v>
       </c>
@@ -2370,8 +2369,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2380,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>95</v>
@@ -2394,10 +2393,10 @@
         <v>62</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>59</v>
@@ -2421,13 +2420,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
@@ -2438,13 +2437,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,10 +2451,10 @@
         <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>68</v>
@@ -2485,9 +2484,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2497,13 +2496,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,10 +2510,10 @@
         <v>70</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -2523,10 +2522,10 @@
         <v>72</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -2535,10 +2534,10 @@
         <v>73</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2547,10 +2546,10 @@
         <v>74</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2559,13 +2558,13 @@
         <v>75</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,13 +2572,13 @@
         <v>76</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,13 +2586,13 @@
         <v>77</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2601,13 +2600,13 @@
         <v>78</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2667,19 +2666,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2687,13 +2687,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>140</v>
+        <v>106</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2704,9 +2707,12 @@
         <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2810,7 +2816,7 @@
         <v>146</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -2829,10 +2835,10 @@
         <v>146</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -2850,13 +2856,13 @@
         <v>146</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>149</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -2873,16 +2879,16 @@
         <v>146</v>
       </c>
       <c r="C7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>149</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -2898,19 +2904,19 @@
         <v>146</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>149</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -2944,9 +2950,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2956,13 +2962,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2970,13 +2976,13 @@
         <v>79</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" s="17"/>
     </row>
@@ -2985,13 +2991,13 @@
         <v>81</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2999,13 +3005,13 @@
         <v>82</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3013,13 +3019,13 @@
         <v>83</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3027,10 +3033,10 @@
         <v>84</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="10"/>
     </row>
@@ -3039,10 +3045,10 @@
         <v>85</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -3051,10 +3057,10 @@
         <v>86</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D8" s="10"/>
     </row>
@@ -3063,10 +3069,10 @@
         <v>87</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D9" s="10"/>
     </row>
@@ -3075,13 +3081,13 @@
         <v>88</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3089,13 +3095,13 @@
         <v>89</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3103,13 +3109,13 @@
         <v>90</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3117,13 +3123,13 @@
         <v>91</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3150,10 +3156,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3162,10 +3168,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>97</v>
@@ -3176,10 +3182,10 @@
         <v>69</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -3190,7 +3196,7 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3244,10 +3250,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,12 +3261,12 @@
         <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>25</v>
@@ -3268,7 +3274,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -3276,7 +3282,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,13 +3308,13 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
@@ -3318,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,7 +3332,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3334,7 +3340,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3342,7 +3348,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3369,7 +3375,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3412,12 +3418,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
@@ -3448,12 +3454,14 @@
       <c r="B2" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="D2" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3461,14 +3469,16 @@
         <v>27</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,13 +3489,13 @@
         <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3512,11 +3522,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3525,16 +3535,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>98</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="49" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3542,13 +3552,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -3559,13 +3569,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -3576,13 +3586,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -3593,13 +3603,13 @@
         <v>34</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
@@ -3610,13 +3620,13 @@
         <v>35</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>1</v>
@@ -3627,13 +3637,13 @@
         <v>37</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
@@ -3663,9 +3673,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3674,10 +3684,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3706,9 +3716,9 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3718,19 +3728,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3738,16 +3748,16 @@
         <v>47</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F2" s="20" t="n">
         <v>0.75</v>
@@ -3769,17 +3779,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1174089068826"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,13 +3800,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,13 +3817,16 @@
         <v>50</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3815,13 +3834,16 @@
         <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3829,11 +3851,14 @@
         <v>54</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>128</v>
+        <v>131</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3860,8 +3885,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3905,8 +3930,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -3916,13 +3941,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3932,7 +3957,7 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3940,10 +3965,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3970,10 +3995,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3982,16 +4007,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,16 +4024,16 @@
         <v>60</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleting copies of block calculation and adjacency graph + changing adjacency calculation
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Template v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,13 +29,14 @@
     <sheet name="Bay Count" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$L$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$E$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="161">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -362,6 +363,9 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left, right, up, down</t>
   </si>
   <si>
     <t xml:space="preserve">Param 1</t>
@@ -844,14 +848,112 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="00FFFFFF"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <border diagonalUp="false" diagonalDown="false">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <diagonal/>
+      </border>
+      <protection locked="true" hidden="false"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="00FFFFFF"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <border diagonalUp="false" diagonalDown="false">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <diagonal/>
+      </border>
+      <protection locked="true" hidden="false"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="00FFFFFF"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <border diagonalUp="false" diagonalDown="false">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <diagonal/>
+      </border>
+      <protection locked="true" hidden="false"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -933,13 +1035,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="86.336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="87.0890688259109"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2344,7 +2446,7 @@
       <c r="M48" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E48"/>
+  <autoFilter ref="A1:L48"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2369,8 +2471,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2379,10 +2481,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>95</v>
@@ -2393,10 +2495,10 @@
         <v>62</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>59</v>
@@ -2426,7 +2528,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
@@ -2437,13 +2539,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,10 +2553,10 @@
         <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>68</v>
@@ -2484,9 +2586,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -2496,13 +2598,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,10 +2612,10 @@
         <v>70</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -2522,10 +2624,10 @@
         <v>72</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -2534,10 +2636,10 @@
         <v>73</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2546,10 +2648,10 @@
         <v>74</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2558,13 +2660,13 @@
         <v>75</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,13 +2674,13 @@
         <v>76</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,13 +2688,13 @@
         <v>77</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,13 +2702,13 @@
         <v>78</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2618,36 +2720,36 @@
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!="Removed"</formula>
     </cfRule>
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!="Built"</formula>
     </cfRule>
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!="Templated"</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A9">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>'Share of Facings'!$T4="Ready"</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>'Share of Facings'!$T4="Removed"</formula>
     </cfRule>
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>'Share of Facings'!$T4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>'Share of Facings'!$T4="Built"</formula>
     </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>'Share of Facings'!$T4="Templated"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>'Share of Facings'!$T4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2674,11 +2776,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2687,13 +2789,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>93</v>
@@ -2704,16 +2806,16 @@
         <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2745,10 +2847,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2775,7 +2877,7 @@
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B3" s="24" t="n">
         <v>1</v>
@@ -2813,10 +2915,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -2832,13 +2934,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -2853,16 +2955,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -2876,19 +2978,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -2901,22 +3003,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -2950,9 +3052,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2962,13 +3064,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2976,13 +3078,13 @@
         <v>79</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F2" s="17"/>
     </row>
@@ -2991,13 +3093,13 @@
         <v>81</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3005,13 +3107,13 @@
         <v>82</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3019,13 +3121,13 @@
         <v>83</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3033,10 +3135,10 @@
         <v>84</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="10"/>
     </row>
@@ -3045,10 +3147,10 @@
         <v>85</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -3057,10 +3159,10 @@
         <v>86</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="10"/>
     </row>
@@ -3069,10 +3171,10 @@
         <v>87</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="10"/>
     </row>
@@ -3081,13 +3183,13 @@
         <v>88</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,13 +3197,13 @@
         <v>89</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3109,13 +3211,13 @@
         <v>90</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3123,13 +3225,13 @@
         <v>91</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3156,10 +3258,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3168,10 +3270,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>97</v>
@@ -3182,10 +3284,10 @@
         <v>69</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -3196,7 +3298,7 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3207,16 +3309,16 @@
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>Purity!$T2="Removed"</formula>
     </cfRule>
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>Purity!$T2="Done"</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>Purity!$T2="Built"</formula>
     </cfRule>
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>Purity!$T2="Templated"</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>Purity!$T2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3250,10 +3352,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,12 +3363,12 @@
         <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>25</v>
@@ -3274,7 +3376,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -3282,7 +3384,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3308,13 +3410,13 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
@@ -3324,7 +3426,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3332,7 +3434,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,7 +3442,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3348,7 +3450,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3375,7 +3477,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3417,13 +3519,13 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
@@ -3495,7 +3597,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3522,11 +3624,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3535,16 +3637,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>98</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="49" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3552,13 +3654,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -3569,13 +3671,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -3586,13 +3688,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -3603,13 +3705,13 @@
         <v>34</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
@@ -3620,13 +3722,13 @@
         <v>35</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>1</v>
@@ -3637,13 +3739,13 @@
         <v>37</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
@@ -3673,9 +3775,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3684,10 +3786,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3716,9 +3818,9 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -3728,19 +3830,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3748,16 +3850,16 @@
         <v>47</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F2" s="20" t="n">
         <v>0.75</v>
@@ -3787,11 +3889,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1174089068826"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3800,16 +3902,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,16 +3919,16 @@
         <v>50</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>104</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,16 +3936,16 @@
         <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,14 +3953,14 @@
         <v>54</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3885,8 +3987,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3930,8 +4032,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -3941,13 +4043,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3957,7 +4059,7 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,10 +4067,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3995,10 +4097,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4007,16 +4109,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4024,16 +4126,16 @@
         <v>60</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>